<commit_message>
updated metadata in 2021 BactAbund, needed to remove a "+" in one of the Treatment names
</commit_message>
<xml_diff>
--- a/Input_Data/week4/144L_2021_BactAbund.xlsx
+++ b/Input_Data/week4/144L_2021_BactAbund.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinealbers/Documents/144l_students_2021/Input_Data/week4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A42F9A46-F9EB-9040-8842-3612D1F1DA57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1AA426-4900-B24C-B123-D8704D38B76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -118,9 +118,6 @@
     <t>Kelp Exudate</t>
   </si>
   <si>
-    <t>Kelp Exudate + NP</t>
-  </si>
-  <si>
     <t>2021-10-05T08:00</t>
   </si>
   <si>
@@ -167,6 +164,9 @@
   </si>
   <si>
     <t>all_cells_uL</t>
+  </si>
+  <si>
+    <t>Kelp Exudate_Nitrate_Phosphate</t>
   </si>
 </sst>
 </file>
@@ -527,12 +527,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB9DCA8-3A58-FF4E-A0AD-EB8E080FD40B}">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q1" sqref="Q1:Q1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="G42" sqref="G42:G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="7" max="7" width="42.33203125" customWidth="1"/>
     <col min="8" max="8" width="25" customWidth="1"/>
     <col min="11" max="11" width="45" customWidth="1"/>
   </cols>
@@ -578,13 +579,13 @@
         <v>21</v>
       </c>
       <c r="N1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="O1" t="s">
         <v>22</v>
       </c>
       <c r="P1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
@@ -619,7 +620,7 @@
         <v>5</v>
       </c>
       <c r="K2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L2" t="b">
         <v>1</v>
@@ -669,7 +670,7 @@
         <v>5</v>
       </c>
       <c r="K3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L3" t="b">
         <v>0</v>
@@ -719,7 +720,7 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L4" t="b">
         <v>0</v>
@@ -769,7 +770,7 @@
         <v>5</v>
       </c>
       <c r="K5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L5" t="b">
         <v>0</v>
@@ -819,7 +820,7 @@
         <v>5</v>
       </c>
       <c r="K6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L6" t="b">
         <v>1</v>
@@ -869,7 +870,7 @@
         <v>5</v>
       </c>
       <c r="K7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L7" t="b">
         <v>0</v>
@@ -919,7 +920,7 @@
         <v>5</v>
       </c>
       <c r="K8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L8" t="b">
         <v>0</v>
@@ -969,7 +970,7 @@
         <v>5</v>
       </c>
       <c r="K9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L9" t="b">
         <v>0</v>
@@ -1019,7 +1020,7 @@
         <v>5</v>
       </c>
       <c r="K10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L10" t="b">
         <v>1</v>
@@ -1069,7 +1070,7 @@
         <v>5</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L11" t="b">
         <v>1</v>
@@ -1119,7 +1120,7 @@
         <v>5</v>
       </c>
       <c r="K12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L12" t="b">
         <v>1</v>
@@ -1169,7 +1170,7 @@
         <v>5</v>
       </c>
       <c r="K13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L13" t="b">
         <v>0</v>
@@ -1219,7 +1220,7 @@
         <v>5</v>
       </c>
       <c r="K14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L14" t="b">
         <v>0</v>
@@ -1269,7 +1270,7 @@
         <v>5</v>
       </c>
       <c r="K15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L15" t="b">
         <v>0</v>
@@ -1319,7 +1320,7 @@
         <v>5</v>
       </c>
       <c r="K16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L16" t="b">
         <v>1</v>
@@ -1369,7 +1370,7 @@
         <v>5</v>
       </c>
       <c r="K17" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L17" t="b">
         <v>0</v>
@@ -1419,7 +1420,7 @@
         <v>5</v>
       </c>
       <c r="K18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L18" t="b">
         <v>0</v>
@@ -1469,7 +1470,7 @@
         <v>5</v>
       </c>
       <c r="K19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L19" t="b">
         <v>0</v>
@@ -1519,7 +1520,7 @@
         <v>5</v>
       </c>
       <c r="K20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L20" t="b">
         <v>1</v>
@@ -1569,7 +1570,7 @@
         <v>5</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L21" t="b">
         <v>1</v>
@@ -1619,7 +1620,7 @@
         <v>5</v>
       </c>
       <c r="K22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L22" t="b">
         <v>1</v>
@@ -1669,7 +1670,7 @@
         <v>5</v>
       </c>
       <c r="K23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L23" t="b">
         <v>0</v>
@@ -1719,7 +1720,7 @@
         <v>5</v>
       </c>
       <c r="K24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L24" t="b">
         <v>0</v>
@@ -1769,7 +1770,7 @@
         <v>5</v>
       </c>
       <c r="K25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L25" t="b">
         <v>0</v>
@@ -1819,7 +1820,7 @@
         <v>5</v>
       </c>
       <c r="K26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L26" t="b">
         <v>1</v>
@@ -1869,7 +1870,7 @@
         <v>5</v>
       </c>
       <c r="K27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L27" t="b">
         <v>0</v>
@@ -1919,7 +1920,7 @@
         <v>5</v>
       </c>
       <c r="K28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L28" t="b">
         <v>0</v>
@@ -1969,7 +1970,7 @@
         <v>5</v>
       </c>
       <c r="K29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L29" t="b">
         <v>0</v>
@@ -2019,7 +2020,7 @@
         <v>5</v>
       </c>
       <c r="K30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L30" t="b">
         <v>1</v>
@@ -2069,7 +2070,7 @@
         <v>5</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L31" t="b">
         <v>1</v>
@@ -2119,7 +2120,7 @@
         <v>5</v>
       </c>
       <c r="K32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L32" t="b">
         <v>1</v>
@@ -2169,7 +2170,7 @@
         <v>5</v>
       </c>
       <c r="K33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L33" t="b">
         <v>0</v>
@@ -2219,7 +2220,7 @@
         <v>5</v>
       </c>
       <c r="K34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L34" t="b">
         <v>0</v>
@@ -2269,7 +2270,7 @@
         <v>5</v>
       </c>
       <c r="K35" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L35" t="b">
         <v>0</v>
@@ -2319,7 +2320,7 @@
         <v>5</v>
       </c>
       <c r="K36" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L36" t="b">
         <v>1</v>
@@ -2369,7 +2370,7 @@
         <v>5</v>
       </c>
       <c r="K37" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L37" t="b">
         <v>0</v>
@@ -2419,7 +2420,7 @@
         <v>5</v>
       </c>
       <c r="K38" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L38" t="b">
         <v>0</v>
@@ -2469,7 +2470,7 @@
         <v>5</v>
       </c>
       <c r="K39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L39" t="b">
         <v>0</v>
@@ -2519,7 +2520,7 @@
         <v>5</v>
       </c>
       <c r="K40" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L40" t="b">
         <v>1</v>
@@ -2569,7 +2570,7 @@
         <v>5</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L41" t="b">
         <v>1</v>
@@ -2607,7 +2608,7 @@
         <v>0</v>
       </c>
       <c r="G42" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H42">
         <v>10</v>
@@ -2619,7 +2620,7 @@
         <v>5</v>
       </c>
       <c r="K42" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L42" t="b">
         <v>1</v>
@@ -2657,19 +2658,19 @@
         <v>1</v>
       </c>
       <c r="G43" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43">
+        <v>10</v>
+      </c>
+      <c r="I43">
+        <v>2</v>
+      </c>
+      <c r="J43">
+        <v>5</v>
+      </c>
+      <c r="K43" t="s">
         <v>27</v>
-      </c>
-      <c r="H43">
-        <v>10</v>
-      </c>
-      <c r="I43">
-        <v>2</v>
-      </c>
-      <c r="J43">
-        <v>5</v>
-      </c>
-      <c r="K43" t="s">
-        <v>28</v>
       </c>
       <c r="L43" t="b">
         <v>0</v>
@@ -2707,7 +2708,7 @@
         <v>2</v>
       </c>
       <c r="G44" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H44">
         <v>10</v>
@@ -2719,7 +2720,7 @@
         <v>5</v>
       </c>
       <c r="K44" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L44" t="b">
         <v>0</v>
@@ -2757,7 +2758,7 @@
         <v>3</v>
       </c>
       <c r="G45" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H45">
         <v>10</v>
@@ -2769,7 +2770,7 @@
         <v>5</v>
       </c>
       <c r="K45" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L45" t="b">
         <v>0</v>
@@ -2807,7 +2808,7 @@
         <v>4</v>
       </c>
       <c r="G46" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H46">
         <v>10</v>
@@ -2819,7 +2820,7 @@
         <v>5</v>
       </c>
       <c r="K46" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L46" t="b">
         <v>1</v>
@@ -2857,7 +2858,7 @@
         <v>5</v>
       </c>
       <c r="G47" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H47">
         <v>10</v>
@@ -2869,7 +2870,7 @@
         <v>5</v>
       </c>
       <c r="K47" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L47" t="b">
         <v>0</v>
@@ -2907,7 +2908,7 @@
         <v>6</v>
       </c>
       <c r="G48" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H48">
         <v>10</v>
@@ -2919,7 +2920,7 @@
         <v>5</v>
       </c>
       <c r="K48" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L48" t="b">
         <v>0</v>
@@ -2957,7 +2958,7 @@
         <v>7</v>
       </c>
       <c r="G49" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H49">
         <v>10</v>
@@ -2969,7 +2970,7 @@
         <v>5</v>
       </c>
       <c r="K49" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L49" t="b">
         <v>0</v>
@@ -3007,7 +3008,7 @@
         <v>8</v>
       </c>
       <c r="G50" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H50">
         <v>10</v>
@@ -3019,7 +3020,7 @@
         <v>5</v>
       </c>
       <c r="K50" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L50" t="b">
         <v>1</v>
@@ -3057,7 +3058,7 @@
         <v>9</v>
       </c>
       <c r="G51" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H51">
         <v>10</v>
@@ -3069,7 +3070,7 @@
         <v>5</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L51" t="b">
         <v>1</v>
@@ -3107,7 +3108,7 @@
         <v>0</v>
       </c>
       <c r="G52" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H52">
         <v>10</v>
@@ -3119,7 +3120,7 @@
         <v>5</v>
       </c>
       <c r="K52" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L52" t="b">
         <v>1</v>
@@ -3157,19 +3158,19 @@
         <v>1</v>
       </c>
       <c r="G53" t="s">
+        <v>43</v>
+      </c>
+      <c r="H53">
+        <v>10</v>
+      </c>
+      <c r="I53">
+        <v>2</v>
+      </c>
+      <c r="J53">
+        <v>5</v>
+      </c>
+      <c r="K53" t="s">
         <v>27</v>
-      </c>
-      <c r="H53">
-        <v>10</v>
-      </c>
-      <c r="I53">
-        <v>2</v>
-      </c>
-      <c r="J53">
-        <v>5</v>
-      </c>
-      <c r="K53" t="s">
-        <v>28</v>
       </c>
       <c r="L53" t="b">
         <v>0</v>
@@ -3207,7 +3208,7 @@
         <v>2</v>
       </c>
       <c r="G54" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H54">
         <v>10</v>
@@ -3219,7 +3220,7 @@
         <v>5</v>
       </c>
       <c r="K54" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L54" t="b">
         <v>0</v>
@@ -3257,7 +3258,7 @@
         <v>3</v>
       </c>
       <c r="G55" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H55">
         <v>10</v>
@@ -3269,7 +3270,7 @@
         <v>5</v>
       </c>
       <c r="K55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L55" t="b">
         <v>0</v>
@@ -3307,7 +3308,7 @@
         <v>4</v>
       </c>
       <c r="G56" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H56">
         <v>10</v>
@@ -3319,7 +3320,7 @@
         <v>5</v>
       </c>
       <c r="K56" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L56" t="b">
         <v>1</v>
@@ -3357,7 +3358,7 @@
         <v>5</v>
       </c>
       <c r="G57" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H57">
         <v>10</v>
@@ -3369,7 +3370,7 @@
         <v>5</v>
       </c>
       <c r="K57" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L57" t="b">
         <v>0</v>
@@ -3407,7 +3408,7 @@
         <v>6</v>
       </c>
       <c r="G58" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H58">
         <v>10</v>
@@ -3419,7 +3420,7 @@
         <v>5</v>
       </c>
       <c r="K58" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L58" t="b">
         <v>0</v>
@@ -3457,7 +3458,7 @@
         <v>7</v>
       </c>
       <c r="G59" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H59">
         <v>10</v>
@@ -3469,7 +3470,7 @@
         <v>5</v>
       </c>
       <c r="K59" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L59" t="b">
         <v>0</v>
@@ -3507,7 +3508,7 @@
         <v>8</v>
       </c>
       <c r="G60" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H60">
         <v>10</v>
@@ -3519,7 +3520,7 @@
         <v>5</v>
       </c>
       <c r="K60" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L60" t="b">
         <v>1</v>
@@ -3557,7 +3558,7 @@
         <v>9</v>
       </c>
       <c r="G61" t="s">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="H61">
         <v>10</v>
@@ -3569,7 +3570,7 @@
         <v>5</v>
       </c>
       <c r="K61" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L61" t="b">
         <v>1</v>
@@ -3619,7 +3620,7 @@
         <v>5</v>
       </c>
       <c r="K62" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L62" t="b">
         <v>1</v>
@@ -3669,7 +3670,7 @@
         <v>5</v>
       </c>
       <c r="K63" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L63" t="b">
         <v>0</v>
@@ -3719,7 +3720,7 @@
         <v>5</v>
       </c>
       <c r="K64" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L64" t="b">
         <v>0</v>
@@ -3769,7 +3770,7 @@
         <v>5</v>
       </c>
       <c r="K65" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L65" t="b">
         <v>0</v>
@@ -3819,7 +3820,7 @@
         <v>5</v>
       </c>
       <c r="K66" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L66" t="b">
         <v>1</v>
@@ -3869,7 +3870,7 @@
         <v>5</v>
       </c>
       <c r="K67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L67" t="b">
         <v>0</v>
@@ -3919,7 +3920,7 @@
         <v>5</v>
       </c>
       <c r="K68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L68" t="b">
         <v>0</v>
@@ -3969,7 +3970,7 @@
         <v>5</v>
       </c>
       <c r="K69" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L69" t="b">
         <v>0</v>
@@ -4019,7 +4020,7 @@
         <v>5</v>
       </c>
       <c r="K70" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L70" t="b">
         <v>1</v>
@@ -4069,7 +4070,7 @@
         <v>5</v>
       </c>
       <c r="K71" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L71" t="b">
         <v>1</v>
@@ -4119,7 +4120,7 @@
         <v>5</v>
       </c>
       <c r="K72" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L72" t="b">
         <v>1</v>
@@ -4169,7 +4170,7 @@
         <v>5</v>
       </c>
       <c r="K73" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="L73" t="b">
         <v>0</v>
@@ -4219,7 +4220,7 @@
         <v>5</v>
       </c>
       <c r="K74" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L74" t="b">
         <v>0</v>
@@ -4269,7 +4270,7 @@
         <v>5</v>
       </c>
       <c r="K75" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L75" t="b">
         <v>0</v>
@@ -4319,7 +4320,7 @@
         <v>5</v>
       </c>
       <c r="K76" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="L76" t="b">
         <v>1</v>
@@ -4369,7 +4370,7 @@
         <v>5</v>
       </c>
       <c r="K77" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="L77" t="b">
         <v>0</v>
@@ -4419,7 +4420,7 @@
         <v>5</v>
       </c>
       <c r="K78" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="L78" t="b">
         <v>0</v>
@@ -4469,7 +4470,7 @@
         <v>5</v>
       </c>
       <c r="K79" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L79" t="b">
         <v>0</v>
@@ -4519,7 +4520,7 @@
         <v>5</v>
       </c>
       <c r="K80" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L80" t="b">
         <v>1</v>
@@ -4569,7 +4570,7 @@
         <v>5</v>
       </c>
       <c r="K81" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L81" t="b">
         <v>1</v>
@@ -4597,8 +4598,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5332B8C1-55B2-BD48-914B-6263445B7F27}">
   <dimension ref="A1:E73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4611,13 +4612,13 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" t="s">
         <v>40</v>
-      </c>
-      <c r="E1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4934,13 +4935,13 @@
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -5121,13 +5122,13 @@
         <v>2</v>
       </c>
       <c r="C31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
@@ -5240,13 +5241,13 @@
         <v>0</v>
       </c>
       <c r="C38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E38" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -5257,13 +5258,13 @@
         <v>1</v>
       </c>
       <c r="C39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -5274,13 +5275,13 @@
         <v>2</v>
       </c>
       <c r="C40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -5427,13 +5428,13 @@
         <v>2</v>
       </c>
       <c r="C49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -5444,13 +5445,13 @@
         <v>3</v>
       </c>
       <c r="C50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -5529,13 +5530,13 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E55" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -5546,13 +5547,13 @@
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E56" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -5597,13 +5598,13 @@
         <v>3</v>
       </c>
       <c r="C59" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D59" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E59" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -5733,13 +5734,13 @@
         <v>2</v>
       </c>
       <c r="C67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E67" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.2">
@@ -5750,13 +5751,13 @@
         <v>3</v>
       </c>
       <c r="C68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E68" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated with DAPI data
</commit_message>
<xml_diff>
--- a/Input_Data/week4/144L_2021_BactAbund.xlsx
+++ b/Input_Data/week4/144L_2021_BactAbund.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinealbers/Documents/144l_students_2021/Input_Data/week4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A1AA426-4900-B24C-B123-D8704D38B76E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0E6DD89-7D34-C242-859E-722097D78BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
+    <workbookView xWindow="-32540" yWindow="-4180" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
-    <sheet name="Data" sheetId="2" r:id="rId2"/>
+    <sheet name="FCM_Data" sheetId="2" r:id="rId2"/>
+    <sheet name="DAPI_Data" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" calcOnSave="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="48">
   <si>
     <t>A</t>
   </si>
@@ -167,6 +168,18 @@
   </si>
   <si>
     <t>Kelp Exudate_Nitrate_Phosphate</t>
+  </si>
+  <si>
+    <t>Cells_mL</t>
+  </si>
+  <si>
+    <t>Cells_mL_Stdev</t>
+  </si>
+  <si>
+    <t>Mean_Biovolume_um3_cell</t>
+  </si>
+  <si>
+    <t>Biovolume_Stdev_um3_cell</t>
   </si>
 </sst>
 </file>
@@ -527,8 +540,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB9DCA8-3A58-FF4E-A0AD-EB8E080FD40B}">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42:G61"/>
+    <sheetView topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5848,4 +5861,279 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C07682-43E0-9749-8711-A66C7C8B7855}">
+  <dimension ref="A1:F13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>660667</v>
+      </c>
+      <c r="D2">
+        <v>73217.755744736962</v>
+      </c>
+      <c r="E2">
+        <v>4.556209250166493E-2</v>
+      </c>
+      <c r="F2">
+        <v>6.0548048518688944E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>919405.58319999999</v>
+      </c>
+      <c r="D3">
+        <v>363326.27392113575</v>
+      </c>
+      <c r="E3">
+        <v>5.0803531793108703E-2</v>
+      </c>
+      <c r="F3">
+        <v>1.1000369174713136E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1133869.7239999999</v>
+      </c>
+      <c r="D4">
+        <v>99930.050143482484</v>
+      </c>
+      <c r="E4">
+        <v>4.0932122992205985E-2</v>
+      </c>
+      <c r="F4">
+        <v>4.684495054588826E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>663088.10880000005</v>
+      </c>
+      <c r="D5">
+        <v>113546.26705004732</v>
+      </c>
+      <c r="E5">
+        <v>3.8714986197324441E-2</v>
+      </c>
+      <c r="F5">
+        <v>5.4464852650337146E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1043597.8280000003</v>
+      </c>
+      <c r="D6">
+        <v>181810.6237172893</v>
+      </c>
+      <c r="E6">
+        <v>6.8116291585186811E-2</v>
+      </c>
+      <c r="F6">
+        <v>1.3492316711132726E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>1115268.2424000003</v>
+      </c>
+      <c r="D7">
+        <v>149497.94850320072</v>
+      </c>
+      <c r="E7">
+        <v>3.2720249084495917E-2</v>
+      </c>
+      <c r="F7">
+        <v>9.6971343755849169E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>672115.29839999997</v>
+      </c>
+      <c r="D8">
+        <v>71870.484141861118</v>
+      </c>
+      <c r="E8">
+        <v>3.6309706278979906E-2</v>
+      </c>
+      <c r="F8">
+        <v>5.0124924763695301E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>1226603.5808000001</v>
+      </c>
+      <c r="D9">
+        <v>153931.80801620887</v>
+      </c>
+      <c r="E9">
+        <v>0.10237022179025781</v>
+      </c>
+      <c r="F9">
+        <v>1.4780122705744487E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>1391554.9543999997</v>
+      </c>
+      <c r="D10">
+        <v>81241.073296844464</v>
+      </c>
+      <c r="E10">
+        <v>6.1333789954676352E-2</v>
+      </c>
+      <c r="F10">
+        <v>9.9273320800025051E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>646948.58800000011</v>
+      </c>
+      <c r="D11">
+        <v>126328.47284772345</v>
+      </c>
+      <c r="E11">
+        <v>5.1854197463218711E-2</v>
+      </c>
+      <c r="F11">
+        <v>9.9434248994746868E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>1665926.8079999995</v>
+      </c>
+      <c r="D12">
+        <v>184066.73734873536</v>
+      </c>
+      <c r="E12">
+        <v>9.5323738342314598E-2</v>
+      </c>
+      <c r="F12">
+        <v>1.3237367101276281E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>1544196.5239999997</v>
+      </c>
+      <c r="D13">
+        <v>116715.17866666666</v>
+      </c>
+      <c r="E13">
+        <v>4.51093985918566E-2</v>
+      </c>
+      <c r="F13">
+        <v>9.7532258357421117E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
modifying bact abundance 2021 to test fetch
</commit_message>
<xml_diff>
--- a/Input_Data/week4/144L_2021_BactAbund.xlsx
+++ b/Input_Data/week4/144L_2021_BactAbund.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinealbers/Documents/144l_students_2021/Input_Data/week4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0E6DD89-7D34-C242-859E-722097D78BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{76390ACE-8606-8747-9F69-F1C3AA85C53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32540" yWindow="-4180" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
+    <workbookView xWindow="-33700" yWindow="-5060" windowWidth="28580" windowHeight="17500" activeTab="4" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="FCM_Data" sheetId="2" r:id="rId2"/>
     <sheet name="DAPI_Data" sheetId="3" r:id="rId3"/>
+    <sheet name="TOC_Data" sheetId="4" r:id="rId4"/>
+    <sheet name="testing fetch" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="50">
   <si>
     <t>A</t>
   </si>
@@ -180,6 +182,12 @@
   </si>
   <si>
     <t>Biovolume_Stdev_um3_cell</t>
+  </si>
+  <si>
+    <t>Kelp_Exudate_Nitrate_Phosphate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">data </t>
   </si>
 </sst>
 </file>
@@ -540,7 +548,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBB9DCA8-3A58-FF4E-A0AD-EB8E080FD40B}">
   <dimension ref="A1:P81"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G62" sqref="G62"/>
     </sheetView>
   </sheetViews>
@@ -5867,270 +5875,465 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0C07682-43E0-9749-8711-A66C7C8B7855}">
   <dimension ref="A1:F13"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+    <col min="4" max="4" width="20.1640625" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>660667</v>
+      </c>
+      <c r="D2">
+        <v>73217.755744736962</v>
+      </c>
+      <c r="E2">
+        <v>4.556209250166493E-2</v>
+      </c>
+      <c r="F2">
+        <v>6.0548048518688944E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>919405.58319999999</v>
+      </c>
+      <c r="D3">
+        <v>363326.27392113575</v>
+      </c>
+      <c r="E3">
+        <v>5.0803531793108703E-2</v>
+      </c>
+      <c r="F3">
+        <v>1.1000369174713136E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>1133869.7239999999</v>
+      </c>
+      <c r="D4">
+        <v>99930.050143482484</v>
+      </c>
+      <c r="E4">
+        <v>4.0932122992205985E-2</v>
+      </c>
+      <c r="F4">
+        <v>4.684495054588826E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>663088.10880000005</v>
+      </c>
+      <c r="D5">
+        <v>113546.26705004732</v>
+      </c>
+      <c r="E5">
+        <v>3.8714986197324441E-2</v>
+      </c>
+      <c r="F5">
+        <v>5.4464852650337146E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>1043597.8280000003</v>
+      </c>
+      <c r="D6">
+        <v>181810.6237172893</v>
+      </c>
+      <c r="E6">
+        <v>6.8116291585186811E-2</v>
+      </c>
+      <c r="F6">
+        <v>1.3492316711132726E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>8</v>
+      </c>
+      <c r="C7">
+        <v>1115268.2424000003</v>
+      </c>
+      <c r="D7">
+        <v>149497.94850320072</v>
+      </c>
+      <c r="E7">
+        <v>3.2720249084495917E-2</v>
+      </c>
+      <c r="F7">
+        <v>9.6971343755849169E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>672115.29839999997</v>
+      </c>
+      <c r="D8">
+        <v>71870.484141861118</v>
+      </c>
+      <c r="E8">
+        <v>3.6309706278979906E-2</v>
+      </c>
+      <c r="F8">
+        <v>5.0124924763695301E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9">
+        <v>4</v>
+      </c>
+      <c r="C9">
+        <v>1226603.5808000001</v>
+      </c>
+      <c r="D9">
+        <v>153931.80801620887</v>
+      </c>
+      <c r="E9">
+        <v>0.10237022179025781</v>
+      </c>
+      <c r="F9">
+        <v>1.4780122705744487E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>1391554.9543999997</v>
+      </c>
+      <c r="D10">
+        <v>81241.073296844464</v>
+      </c>
+      <c r="E10">
+        <v>6.1333789954676352E-2</v>
+      </c>
+      <c r="F10">
+        <v>9.9273320800025051E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>646948.58800000011</v>
+      </c>
+      <c r="D11">
+        <v>126328.47284772345</v>
+      </c>
+      <c r="E11">
+        <v>5.1854197463218711E-2</v>
+      </c>
+      <c r="F11">
+        <v>9.9434248994746868E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>1665926.8079999995</v>
+      </c>
+      <c r="D12">
+        <v>184066.73734873536</v>
+      </c>
+      <c r="E12">
+        <v>9.5323738342314598E-2</v>
+      </c>
+      <c r="F12">
+        <v>1.3237367101276281E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>1544196.5239999997</v>
+      </c>
+      <c r="D13">
+        <v>116715.17866666666</v>
+      </c>
+      <c r="E13">
+        <v>4.51093985918566E-2</v>
+      </c>
+      <c r="F13">
+        <v>9.7532258357421117E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A06D71C-2B86-EB48-85FD-54A340C7E5B0}">
+  <dimension ref="A1:B17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23CE69D4-53EC-E749-9B61-CCD69471A578}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>660667</v>
-      </c>
-      <c r="D2">
-        <v>73217.755744736962</v>
-      </c>
-      <c r="E2">
-        <v>4.556209250166493E-2</v>
-      </c>
-      <c r="F2">
-        <v>6.0548048518688944E-3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3">
-        <v>4</v>
-      </c>
-      <c r="C3">
-        <v>919405.58319999999</v>
-      </c>
-      <c r="D3">
-        <v>363326.27392113575</v>
-      </c>
-      <c r="E3">
-        <v>5.0803531793108703E-2</v>
-      </c>
-      <c r="F3">
-        <v>1.1000369174713136E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>8</v>
-      </c>
-      <c r="C4">
-        <v>1133869.7239999999</v>
-      </c>
-      <c r="D4">
-        <v>99930.050143482484</v>
-      </c>
-      <c r="E4">
-        <v>4.0932122992205985E-2</v>
-      </c>
-      <c r="F4">
-        <v>4.684495054588826E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>663088.10880000005</v>
-      </c>
-      <c r="D5">
-        <v>113546.26705004732</v>
-      </c>
-      <c r="E5">
-        <v>3.8714986197324441E-2</v>
-      </c>
-      <c r="F5">
-        <v>5.4464852650337146E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>1043597.8280000003</v>
-      </c>
-      <c r="D6">
-        <v>181810.6237172893</v>
-      </c>
-      <c r="E6">
-        <v>6.8116291585186811E-2</v>
-      </c>
-      <c r="F6">
-        <v>1.3492316711132726E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>1115268.2424000003</v>
-      </c>
-      <c r="D7">
-        <v>149497.94850320072</v>
-      </c>
-      <c r="E7">
-        <v>3.2720249084495917E-2</v>
-      </c>
-      <c r="F7">
-        <v>9.6971343755849169E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>672115.29839999997</v>
-      </c>
-      <c r="D8">
-        <v>71870.484141861118</v>
-      </c>
-      <c r="E8">
-        <v>3.6309706278979906E-2</v>
-      </c>
-      <c r="F8">
-        <v>5.0124924763695301E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>43</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>1226603.5808000001</v>
-      </c>
-      <c r="D9">
-        <v>153931.80801620887</v>
-      </c>
-      <c r="E9">
-        <v>0.10237022179025781</v>
-      </c>
-      <c r="F9">
-        <v>1.4780122705744487E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10">
-        <v>8</v>
-      </c>
-      <c r="C10">
-        <v>1391554.9543999997</v>
-      </c>
-      <c r="D10">
-        <v>81241.073296844464</v>
-      </c>
-      <c r="E10">
-        <v>6.1333789954676352E-2</v>
-      </c>
-      <c r="F10">
-        <v>9.9273320800025051E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>646948.58800000011</v>
-      </c>
-      <c r="D11">
-        <v>126328.47284772345</v>
-      </c>
-      <c r="E11">
-        <v>5.1854197463218711E-2</v>
-      </c>
-      <c r="F11">
-        <v>9.9434248994746868E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12">
-        <v>1665926.8079999995</v>
-      </c>
-      <c r="D12">
-        <v>184066.73734873536</v>
-      </c>
-      <c r="E12">
-        <v>9.5323738342314598E-2</v>
-      </c>
-      <c r="F12">
-        <v>1.3237367101276281E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13">
-        <v>8</v>
-      </c>
-      <c r="C13">
-        <v>1544196.5239999997</v>
-      </c>
-      <c r="D13">
-        <v>116715.17866666666</v>
-      </c>
-      <c r="E13">
-        <v>4.51093985918566E-2</v>
-      </c>
-      <c r="F13">
-        <v>9.7532258357421117E-3</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing bact abundance for testing again
</commit_message>
<xml_diff>
--- a/Input_Data/week4/144L_2021_BactAbund.xlsx
+++ b/Input_Data/week4/144L_2021_BactAbund.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justinealbers/Documents/144l_students_2021/Input_Data/week4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76390ACE-8606-8747-9F69-F1C3AA85C53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F140BFBC-27BD-C343-BECD-FD5CB4908238}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33700" yWindow="-5060" windowWidth="28580" windowHeight="17500" activeTab="4" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
+    <workbookView xWindow="-33700" yWindow="-5060" windowWidth="28580" windowHeight="17500" activeTab="3" xr2:uid="{F709D6EC-9781-194F-92A9-3A8FA05D336F}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="FCM_Data" sheetId="2" r:id="rId2"/>
     <sheet name="DAPI_Data" sheetId="3" r:id="rId3"/>
     <sheet name="TOC_Data" sheetId="4" r:id="rId4"/>
-    <sheet name="testing fetch" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="49">
   <si>
     <t>A</t>
   </si>
@@ -185,9 +184,6 @@
   </si>
   <si>
     <t>Kelp_Exudate_Nitrate_Phosphate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">data </t>
   </si>
 </sst>
 </file>
@@ -6156,7 +6152,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A06D71C-2B86-EB48-85FD-54A340C7E5B0}">
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
@@ -6304,39 +6300,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23CE69D4-53EC-E749-9B61-CCD69471A578}">
-  <dimension ref="A1:A4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>